<commit_message>
lots of changes and new files for nsrdb
</commit_message>
<xml_diff>
--- a/Macmillan_Committee_Form.xlsx
+++ b/Macmillan_Committee_Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tulay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\AES\Student\Fall 2019 cohort 1\Cohort 1 PhDs\Madeline Macmillan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD78610-AE83-414B-A652-896FB8103E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28CF8649-E120-418C-B9D5-04C8C14A98D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="1485" windowWidth="14400" windowHeight="7365" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Committee Advisor Form" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Committee Advisor Form'!$A$1:$J$40</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="154">
   <si>
     <t>Minor Program:</t>
   </si>
@@ -1802,66 +1802,193 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1896,199 +2023,72 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2339,7 +2339,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Advisor </a:t>
@@ -2426,7 +2425,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Member</a:t>
@@ -2513,7 +2511,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Member</a:t>
@@ -2600,7 +2597,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Co-Advisor</a:t>
@@ -2687,7 +2683,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Remove </a:t>
@@ -2774,7 +2769,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Remove </a:t>
@@ -2861,7 +2855,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Minor Representative:                      Voting member</a:t>
@@ -2936,7 +2929,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Change Advisor Before Committee Established</a:t>
@@ -3011,7 +3003,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Change Existing Committee or             Advisor After Committee Established </a:t>
@@ -3098,7 +3089,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Non-voting member</a:t>
@@ -3185,7 +3175,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Non-voting member</a:t>
@@ -3260,7 +3249,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Establish Initial Committee</a:t>
@@ -3335,7 +3323,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t> Add Co-Advisor or Minor Rep          Before Committee Established</a:t>
@@ -3422,7 +3409,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Voting member</a:t>
@@ -3509,7 +3495,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Existing Co-Advisor</a:t>
@@ -3596,7 +3581,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Existing Member</a:t>
@@ -3683,7 +3667,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Existing Member</a:t>
@@ -3770,7 +3753,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Existing Advisor </a:t>
@@ -3857,7 +3839,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Voting member</a:t>
@@ -3944,7 +3925,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Add Chairperson</a:t>
@@ -4031,7 +4011,6 @@
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Segoe UI"/>
-                  <a:ea typeface="Segoe UI"/>
                   <a:cs typeface="Segoe UI"/>
                 </a:rPr>
                 <a:t>Existing Chair</a:t>
@@ -4044,6 +4023,76 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F9B0D9-35B3-4197-A299-97A4AEB6BBAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1403350" y="1054100"/>
+          <a:ext cx="2190750" cy="215900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Advanced Energy Systems</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4353,7 +4402,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4397,7 +4446,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4422,15 +4471,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" customWidth="1"/>
@@ -4445,18 +4494,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
       <c r="K1" s="61" t="s">
         <v>12</v>
       </c>
@@ -4465,18 +4514,18 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="115" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
+      <c r="J2" s="115"/>
       <c r="K2" s="62" t="s">
         <v>116</v>
       </c>
@@ -4489,18 +4538,18 @@
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
       <c r="K3" s="58" t="s">
         <v>18</v>
       </c>
@@ -4516,18 +4565,18 @@
       <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="117" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="119" t="s">
+      <c r="D4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="121" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
       <c r="K4" s="58" t="s">
         <v>19</v>
       </c>
@@ -4546,19 +4595,19 @@
       <c r="B5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="120" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
       <c r="H5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="125">
+      <c r="I5" s="96">
         <v>10721204</v>
       </c>
-      <c r="J5" s="126"/>
+      <c r="J5" s="97"/>
       <c r="K5" s="59" t="s">
         <v>16</v>
       </c>
@@ -4578,19 +4627,17 @@
       <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="127" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="127"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
       <c r="H6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="131" t="s">
+      <c r="I6" s="102" t="s">
         <v>144</v>
       </c>
-      <c r="J6" s="132"/>
+      <c r="J6" s="103"/>
       <c r="K6" s="59" t="s">
         <v>101</v>
       </c>
@@ -4610,19 +4657,19 @@
       <c r="B7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="127"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
       <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="104" t="s">
         <v>145</v>
       </c>
-      <c r="J7" s="133"/>
+      <c r="J7" s="104"/>
       <c r="K7" s="57" t="s">
         <v>22</v>
       </c>
@@ -4662,19 +4709,19 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="134" t="s">
+      <c r="A9" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="134"/>
-      <c r="C9" s="135"/>
-      <c r="D9" s="135"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
       <c r="F9" s="31"/>
-      <c r="G9" s="136" t="s">
+      <c r="G9" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
-      <c r="J9" s="136"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="107"/>
       <c r="K9" s="57" t="s">
         <v>23</v>
       </c>
@@ -4694,10 +4741,10 @@
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
       <c r="F10" s="31"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="137"/>
-      <c r="I10" s="137"/>
-      <c r="J10" s="137"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="108"/>
       <c r="K10" s="59" t="s">
         <v>24</v>
       </c>
@@ -4712,18 +4759,18 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="129"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="130"/>
+      <c r="B11" s="100"/>
+      <c r="C11" s="100"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="100"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="101"/>
       <c r="K11" s="59" t="s">
         <v>25</v>
       </c>
@@ -4739,20 +4786,20 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="93" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122"/>
-      <c r="E12" s="122"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="123"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="94"/>
       <c r="K12" s="57" t="s">
         <v>31</v>
       </c>
@@ -4768,18 +4815,18 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="138"/>
-      <c r="B13" s="140" t="s">
+      <c r="A13" s="110"/>
+      <c r="B13" s="112" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="113"/>
       <c r="K13" s="59" t="s">
         <v>102</v>
       </c>
@@ -4795,21 +4842,21 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="139"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="101" t="s">
+      <c r="C14" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="101"/>
+      <c r="D14" s="75"/>
       <c r="E14" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="101" t="s">
+      <c r="F14" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="G14" s="101"/>
+      <c r="G14" s="75"/>
       <c r="H14" s="29" t="s">
         <v>74</v>
       </c>
@@ -4830,20 +4877,20 @@
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" s="7" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="107"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="85"/>
       <c r="K15" s="59" t="s">
         <v>104</v>
       </c>
@@ -4859,21 +4906,21 @@
       <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:15" s="7" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="70"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="101" t="s">
+      <c r="C16" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="101"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="101" t="s">
+      <c r="F16" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="G16" s="101"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="29" t="s">
         <v>74</v>
       </c>
@@ -4896,20 +4943,20 @@
       <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:19" s="7" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="84" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="107"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="85"/>
       <c r="K17" s="59" t="s">
         <v>106</v>
       </c>
@@ -4925,21 +4972,21 @@
       <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:19" s="7" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
+      <c r="A18" s="124"/>
       <c r="B18" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="75" t="s">
         <v>147</v>
       </c>
-      <c r="D18" s="101"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="101"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="29" t="s">
         <v>74</v>
       </c>
@@ -4962,20 +5009,20 @@
       <c r="O18" s="8"/>
     </row>
     <row r="19" spans="1:19" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="138" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="99"/>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
-      <c r="J19" s="100"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="138"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="139"/>
       <c r="K19" s="59" t="s">
         <v>108</v>
       </c>
@@ -4988,23 +5035,27 @@
       <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:19" s="7" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="101"/>
+      <c r="D20" s="75"/>
       <c r="E20" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
+      <c r="F20" s="75" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="75"/>
       <c r="H20" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="I20" s="54"/>
+      <c r="I20" s="54" t="s">
+        <v>152</v>
+      </c>
       <c r="J20" s="21"/>
       <c r="K20" s="57" t="s">
         <v>35</v>
@@ -5017,20 +5068,20 @@
       <c r="S20" s="64"/>
     </row>
     <row r="21" spans="1:19" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="110" t="s">
+      <c r="B21" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="111"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="125"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="126"/>
       <c r="K21" s="57" t="s">
         <v>10</v>
       </c>
@@ -5041,19 +5092,19 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:19" s="7" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="70"/>
+      <c r="A22" s="124"/>
       <c r="B22" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="101" t="s">
+      <c r="C22" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="101"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
       <c r="H22" s="29" t="s">
         <v>74</v>
       </c>
@@ -5070,20 +5121,20 @@
       <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:19" s="7" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="106"/>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="106"/>
-      <c r="J23" s="107"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="85"/>
       <c r="K23" s="59" t="s">
         <v>109</v>
       </c>
@@ -5095,19 +5146,21 @@
       <c r="O23" s="8"/>
     </row>
     <row r="24" spans="1:19" s="7" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="101" t="s">
+      <c r="C24" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="101"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
+      <c r="F24" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="75"/>
       <c r="H24" s="29" t="s">
         <v>74</v>
       </c>
@@ -5124,20 +5177,20 @@
       <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:19" s="7" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="108" t="s">
+      <c r="A25" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B25" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="C25" s="106"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="106"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="106"/>
-      <c r="J25" s="107"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="85"/>
       <c r="K25" s="59" t="s">
         <v>110</v>
       </c>
@@ -5150,17 +5203,17 @@
       <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:19" s="7" customFormat="1" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="109"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
       <c r="E26" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
       <c r="H26" s="29" t="s">
         <v>74</v>
       </c>
@@ -5177,20 +5230,20 @@
       <c r="O26" s="8"/>
     </row>
     <row r="27" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="107"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="85"/>
       <c r="K27" s="59" t="s">
         <v>111</v>
       </c>
@@ -5201,17 +5254,17 @@
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="109"/>
+      <c r="A28" s="72"/>
       <c r="B28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
       <c r="H28" s="29" t="s">
         <v>74</v>
       </c>
@@ -5225,18 +5278,18 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="152" t="s">
+      <c r="A29" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="153"/>
-      <c r="C29" s="153"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="153"/>
-      <c r="G29" s="153"/>
-      <c r="H29" s="153"/>
-      <c r="I29" s="153"/>
-      <c r="J29" s="154"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="83"/>
       <c r="K29" s="60" t="s">
         <v>98</v>
       </c>
@@ -5245,20 +5298,20 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="148" t="s">
+      <c r="A30" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="149"/>
-      <c r="C30" s="150" t="s">
+      <c r="B30" s="78"/>
+      <c r="C30" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="150"/>
-      <c r="J30" s="151"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="66" t="s">
         <v>135</v>
       </c>
@@ -5267,18 +5320,18 @@
       </c>
     </row>
     <row r="31" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="148" t="s">
         <v>131</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="76"/>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="149"/>
+      <c r="I31" s="149"/>
+      <c r="J31" s="150"/>
       <c r="K31" s="59" t="s">
         <v>99</v>
       </c>
@@ -5287,17 +5340,17 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="156" t="s">
+      <c r="A32" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="157"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="151"/>
+      <c r="D32" s="151"/>
       <c r="E32" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
+      <c r="F32" s="152"/>
+      <c r="G32" s="152"/>
       <c r="H32" s="63" t="s">
         <v>74</v>
       </c>
@@ -5312,37 +5365,37 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:12" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="145" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="147"/>
-      <c r="D33" s="147"/>
-      <c r="E33" s="80" t="s">
+      <c r="B33" s="146"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="80"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="82"/>
+      <c r="F33" s="154"/>
+      <c r="G33" s="154"/>
+      <c r="H33" s="155"/>
+      <c r="I33" s="155"/>
+      <c r="J33" s="156"/>
       <c r="L33" s="57" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="83" t="s">
+      <c r="A34" s="157" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="84"/>
-      <c r="G34" s="84"/>
-      <c r="H34" s="84"/>
-      <c r="I34" s="84"/>
-      <c r="J34" s="85"/>
+      <c r="B34" s="158"/>
+      <c r="C34" s="158"/>
+      <c r="D34" s="158"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="158"/>
+      <c r="H34" s="158"/>
+      <c r="I34" s="158"/>
+      <c r="J34" s="159"/>
       <c r="K34" s="59"/>
       <c r="L34" s="57" t="s">
         <v>15</v>
@@ -5352,14 +5405,14 @@
       <c r="A35" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="145"/>
-      <c r="C35" s="146"/>
+      <c r="B35" s="73"/>
+      <c r="C35" s="74"/>
       <c r="D35" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="155"/>
-      <c r="F35" s="155"/>
-      <c r="G35" s="155"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="29" t="s">
         <v>74</v>
       </c>
@@ -5374,14 +5427,14 @@
       <c r="A36" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="145"/>
-      <c r="C36" s="146"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="74"/>
       <c r="D36" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
+      <c r="E36" s="153"/>
+      <c r="F36" s="153"/>
+      <c r="G36" s="153"/>
       <c r="H36" s="29" t="s">
         <v>74</v>
       </c>
@@ -5393,27 +5446,27 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="71" t="s">
+      <c r="A37" s="145" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="72"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37" s="80" t="s">
+      <c r="B37" s="146"/>
+      <c r="C37" s="147"/>
+      <c r="D37" s="147"/>
+      <c r="E37" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="F37" s="80"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="87"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="154"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="160"/>
+      <c r="J37" s="161"/>
       <c r="K37" s="59"/>
       <c r="L37" s="60" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="103" t="s">
+      <c r="A38" s="141" t="s">
         <v>127</v>
       </c>
       <c r="B38" s="32" t="s">
@@ -5439,11 +5492,11 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="104"/>
-      <c r="B39" s="68" t="s">
+      <c r="A39" s="142"/>
+      <c r="B39" s="144" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="68"/>
+      <c r="C39" s="144"/>
       <c r="D39" s="34" t="s">
         <v>39</v>
       </c>
@@ -5463,11 +5516,11 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="105"/>
-      <c r="B40" s="161" t="s">
+      <c r="A40" s="143"/>
+      <c r="B40" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="161"/>
+      <c r="C40" s="92"/>
       <c r="D40" s="41" t="s">
         <v>55</v>
       </c>
@@ -5482,163 +5535,163 @@
       <c r="K40" s="59"/>
     </row>
     <row r="41" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="158" t="s">
+      <c r="A41" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="159"/>
-      <c r="C41" s="159"/>
-      <c r="D41" s="159"/>
-      <c r="E41" s="159"/>
-      <c r="F41" s="159"/>
-      <c r="G41" s="159"/>
-      <c r="H41" s="159"/>
-      <c r="I41" s="159"/>
-      <c r="J41" s="160"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="90"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="91"/>
       <c r="K41" s="59"/>
     </row>
     <row r="42" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="133" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="95"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="96"/>
+      <c r="B42" s="134"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
+      <c r="E42" s="134"/>
+      <c r="F42" s="134"/>
+      <c r="G42" s="134"/>
+      <c r="H42" s="134"/>
+      <c r="I42" s="134"/>
+      <c r="J42" s="135"/>
       <c r="K42" s="60"/>
     </row>
     <row r="43" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="97" t="s">
+      <c r="A43" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
-      <c r="I43" s="98"/>
-      <c r="J43" s="98"/>
+      <c r="B43" s="137"/>
+      <c r="C43" s="137"/>
+      <c r="D43" s="137"/>
+      <c r="E43" s="137"/>
+      <c r="F43" s="137"/>
+      <c r="G43" s="137"/>
+      <c r="H43" s="137"/>
+      <c r="I43" s="137"/>
+      <c r="J43" s="137"/>
       <c r="K43" s="60"/>
     </row>
     <row r="44" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="102" t="s">
+      <c r="A44" s="140" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="98"/>
-      <c r="C44" s="98"/>
-      <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="98"/>
-      <c r="G44" s="98"/>
-      <c r="H44" s="98"/>
-      <c r="I44" s="98"/>
-      <c r="J44" s="98"/>
+      <c r="B44" s="137"/>
+      <c r="C44" s="137"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="137"/>
+      <c r="J44" s="137"/>
       <c r="K44" s="59"/>
     </row>
     <row r="45" spans="1:12" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="88" t="s">
+      <c r="A45" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="89"/>
-      <c r="C45" s="89"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="89"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="90"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="128"/>
+      <c r="I45" s="128"/>
+      <c r="J45" s="129"/>
       <c r="K45" s="59"/>
     </row>
     <row r="46" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="89"/>
-      <c r="E46" s="89"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="89"/>
-      <c r="J46" s="90"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="128"/>
+      <c r="E46" s="128"/>
+      <c r="F46" s="128"/>
+      <c r="G46" s="128"/>
+      <c r="H46" s="128"/>
+      <c r="I46" s="128"/>
+      <c r="J46" s="129"/>
     </row>
     <row r="47" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="88" t="s">
+      <c r="A47" s="127" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="89"/>
-      <c r="C47" s="89"/>
-      <c r="D47" s="89"/>
-      <c r="E47" s="89"/>
-      <c r="F47" s="89"/>
-      <c r="G47" s="89"/>
-      <c r="H47" s="89"/>
-      <c r="I47" s="89"/>
-      <c r="J47" s="90"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="128"/>
+      <c r="E47" s="128"/>
+      <c r="F47" s="128"/>
+      <c r="G47" s="128"/>
+      <c r="H47" s="128"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="129"/>
     </row>
     <row r="48" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="127" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="92"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="92"/>
-      <c r="J48" s="93"/>
+      <c r="B48" s="131"/>
+      <c r="C48" s="131"/>
+      <c r="D48" s="131"/>
+      <c r="E48" s="131"/>
+      <c r="F48" s="131"/>
+      <c r="G48" s="131"/>
+      <c r="H48" s="131"/>
+      <c r="I48" s="131"/>
+      <c r="J48" s="132"/>
     </row>
     <row r="49" spans="1:12" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="88" t="s">
+      <c r="A49" s="127" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="89"/>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="90"/>
+      <c r="B49" s="128"/>
+      <c r="C49" s="128"/>
+      <c r="D49" s="128"/>
+      <c r="E49" s="128"/>
+      <c r="F49" s="128"/>
+      <c r="G49" s="128"/>
+      <c r="H49" s="128"/>
+      <c r="I49" s="128"/>
+      <c r="J49" s="129"/>
     </row>
     <row r="50" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="88" t="s">
+      <c r="A50" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="89"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="89"/>
-      <c r="J50" s="90"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="128"/>
+      <c r="E50" s="128"/>
+      <c r="F50" s="128"/>
+      <c r="G50" s="128"/>
+      <c r="H50" s="128"/>
+      <c r="I50" s="128"/>
+      <c r="J50" s="129"/>
     </row>
     <row r="51" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
+      <c r="A51" s="130" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="91"/>
-      <c r="G51" s="91"/>
-      <c r="H51" s="91"/>
-      <c r="I51" s="91"/>
-      <c r="J51" s="91"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="130"/>
+      <c r="D51" s="130"/>
+      <c r="E51" s="130"/>
+      <c r="F51" s="130"/>
+      <c r="G51" s="130"/>
+      <c r="H51" s="130"/>
+      <c r="I51" s="130"/>
+      <c r="J51" s="130"/>
     </row>
     <row r="52" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="67" t="s">
@@ -5646,18 +5699,18 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="48.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="142" t="s">
+      <c r="A53" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="143"/>
-      <c r="C53" s="143"/>
-      <c r="D53" s="143"/>
-      <c r="E53" s="143"/>
-      <c r="F53" s="143"/>
-      <c r="G53" s="143"/>
-      <c r="H53" s="143"/>
-      <c r="I53" s="143"/>
-      <c r="J53" s="144"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="69"/>
+      <c r="J53" s="70"/>
     </row>
     <row r="54" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5891,6 +5944,74 @@
   <sheetProtection algorithmName="SHA-512" hashValue="qPVenHYEfEwWC1OHzflTxTMrGDdlgiry0eZ3MY3GY/3KPrXWfwqloy//EcMXdD/pblIKfsGjEaSWnogjgWU/cw==" saltValue="FsixGk1YIRPCIAjxzibYaw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="84">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A50:J50"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G9:J10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B13:J13"/>
     <mergeCell ref="A53:J53"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B35:C35"/>
@@ -5907,74 +6028,6 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A41:J41"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:J10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="A47:J47"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A44:J44"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:J37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations xWindow="1929" yWindow="642" count="7">

</xml_diff>